<commit_message>
deathline 27 maart crud gemaakt + alles in database
</commit_message>
<xml_diff>
--- a/databaseles/php.xlsx
+++ b/databaseles/php.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Periode 3\PHP\PHPP1\databaseles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B8DF9D-4965-4F98-870C-71F91A76062C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042064DF-2D45-4725-B1F5-50110CC4742B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D2A127AB-232A-43A2-935B-8B938D990DB4}"/>
+    <workbookView xWindow="18036" yWindow="5304" windowWidth="17280" windowHeight="8964" xr2:uid="{D2A127AB-232A-43A2-935B-8B938D990DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>Productnaam</t>
   </si>
@@ -49,13 +49,124 @@
   </si>
   <si>
     <t>Categorie</t>
+  </si>
+  <si>
+    <t>Nike Am 97 Celebration Of The Swoosh Cos</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>Heren schoenen</t>
+  </si>
+  <si>
+    <t>Jordan 1 Mid</t>
+  </si>
+  <si>
+    <t>Mooie groene schoenen</t>
+  </si>
+  <si>
+    <t>Mooie witte schoenen</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>Vans Authentic</t>
+  </si>
+  <si>
+    <t>Mooie grijze schoenen</t>
+  </si>
+  <si>
+    <t>gray</t>
+  </si>
+  <si>
+    <t>Buffalo Crevis</t>
+  </si>
+  <si>
+    <t>pink</t>
+  </si>
+  <si>
+    <t>Mooie roze schoenen</t>
+  </si>
+  <si>
+    <t>Nike Air Max 2090</t>
+  </si>
+  <si>
+    <t>Nike Air Max 270</t>
+  </si>
+  <si>
+    <t>Mooie zwarte schoenen</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>adidas Ozweego Suede</t>
+  </si>
+  <si>
+    <t>Kinder schoenen</t>
+  </si>
+  <si>
+    <t>Nike Air Force 1</t>
+  </si>
+  <si>
+    <t>Nike Tuned 1</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/nike-tuned-1-baby-schoenen-82855?v=316161003104#!searchCategory=kids</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/nike-air-force-1-basisschool-schoenen-7926?v=316701113504#!searchCategory=kids/tieners/schoenen</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/adidas-ozweego-suede-voorschools-schoenen-89995?v=316478400704#!searchCategory=kids/kinderen/schoenen</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/nike-air-max-270-dames-schoenen-50034?v=315240221002#!searchCategory=alle</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/nike-air-max-2090-dames-schoenen-82539?v=315240847202#!searchCategory=vrouwen/schoenen/running</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/buffalo-crevis-dames-schoenen-97731?v=315241136902#!searchCategory=vrouwen/schoenen/casual</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/jordan-1-mid-heren-schoenen-49357?v=314101010404#!searchCategory=heren/schoenen</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/vans-authentic-heren-schoenen-43758?v=314520452104#!searchCategory=heren/schoenen/canvasskate</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/nike-am-97-celebration-of-the-swoosh-cos-basisschool-schoenen-84468</t>
+  </si>
+  <si>
+    <t>Dames schoenen</t>
+  </si>
+  <si>
+    <t>Baby schoenen</t>
+  </si>
+  <si>
+    <t>https://www.footlocker.nl/nl/p/nike-air-force-1-highness-baby-schoenen-82803?v=316160928004#!searchCategory=kids/baby/schoenen</t>
+  </si>
+  <si>
+    <t>Mooie paarse schoenen</t>
+  </si>
+  <si>
+    <t>Nike Air Force 1 Highness</t>
+  </si>
+  <si>
+    <t>paars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +178,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -89,14 +208,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,42 +546,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E20EFE-B67F-440C-A476-626A60AB4D68}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
     <col min="5" max="5" width="8.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4">
+        <v>119.99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6">
+        <v>500</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6">
+        <v>600</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4">
+        <v>79.989999999999995</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="6">
+        <v>650</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4">
+        <v>99.99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6">
+        <v>800</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>149.99</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="6">
+        <v>600</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4">
+        <v>149.99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6">
+        <v>850</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
+        <v>64.989999999999995</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="6">
+        <v>400</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="4">
+        <v>84.99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="6">
+        <v>450</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4">
+        <v>59.99</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="6">
+        <v>150</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11">
+        <v>54.99</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="6">
+        <v>150</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G10" r:id="rId1" location="!searchCategory=kids" display="https://www.footlocker.nl/nl/p/nike-tuned-1-baby-schoenen-82855?v=316161003104 - !searchCategory=kids" xr:uid="{52B36600-F95D-45DB-B2A0-D950C6EC116F}"/>
+    <hyperlink ref="G9" r:id="rId2" location="!searchCategory=kids/tieners/schoenen" display="https://www.footlocker.nl/nl/p/nike-air-force-1-basisschool-schoenen-7926?v=316701113504 - !searchCategory=kids/tieners/schoenen" xr:uid="{46A2DA2E-202E-428D-BD22-9B96D4784872}"/>
+    <hyperlink ref="G8" r:id="rId3" location="!searchCategory=kids/kinderen/schoenen" xr:uid="{D6ECCFAD-8ED3-4A1F-BF51-0DC9DA90C13E}"/>
+    <hyperlink ref="G7" r:id="rId4" location="!searchCategory=alle" xr:uid="{6BA771F6-BAB3-422A-AF93-234F6CD5C293}"/>
+    <hyperlink ref="G6" r:id="rId5" location="!searchCategory=vrouwen/schoenen/running" display="!searchCategory=vrouwen/schoenen/running" xr:uid="{95062A60-0033-4267-B22E-958A3136F1B5}"/>
+    <hyperlink ref="G5" r:id="rId6" location="!searchCategory=vrouwen/schoenen/casual" display="https://www.footlocker.nl/nl/p/buffalo-crevis-dames-schoenen-97731?v=315241136902 - !searchCategory=vrouwen/schoenen/casual" xr:uid="{3CC346F7-F659-4480-8383-E44C006E802F}"/>
+    <hyperlink ref="G2" r:id="rId7" location="!searchCategory=heren/schoenen" display="https://www.footlocker.nl/nl/p/jordan-1-mid-heren-schoenen-49357?v=314101010404 - !searchCategory=heren/schoenen" xr:uid="{E7227B9C-7930-4013-B25A-9BCBE14E629C}"/>
+    <hyperlink ref="G4" r:id="rId8" location="!searchCategory=heren/schoenen/canvasskate" display="https://www.footlocker.nl/nl/p/vans-authentic-heren-schoenen-43758?v=314520452104 - !searchCategory=heren/schoenen/canvasskate" xr:uid="{073E643B-A882-423B-B531-4B67BBF9A05D}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{CA662558-37A1-48C0-84E9-8E7D1D751590}"/>
+    <hyperlink ref="G11" r:id="rId10" location="!searchCategory=kids/baby/schoenen" display="https://www.footlocker.nl/nl/p/nike-air-force-1-highness-baby-schoenen-82803?v=316160928004 - !searchCategory=kids/baby/schoenen" xr:uid="{79864D07-5CD5-489F-BF6B-48789F0BCFA9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added other files + Updated product excel sheet
</commit_message>
<xml_diff>
--- a/databaseles/php.xlsx
+++ b/databaseles/php.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Periode 3\PHP\PHPP1\databaseles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042064DF-2D45-4725-B1F5-50110CC4742B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{802429BB-F726-41CC-BCDC-67FC8FE97FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18036" yWindow="5304" windowWidth="17280" windowHeight="8964" xr2:uid="{D2A127AB-232A-43A2-935B-8B938D990DB4}"/>
+    <workbookView xWindow="6684" yWindow="2628" windowWidth="17280" windowHeight="8964" xr2:uid="{D2A127AB-232A-43A2-935B-8B938D990DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Productnaam</t>
   </si>
@@ -160,6 +160,39 @@
   </si>
   <si>
     <t>paars</t>
+  </si>
+  <si>
+    <t>Picture Name</t>
+  </si>
+  <si>
+    <t>j1.png</t>
+  </si>
+  <si>
+    <t>am1.png</t>
+  </si>
+  <si>
+    <t>v1.png</t>
+  </si>
+  <si>
+    <t>n1.png</t>
+  </si>
+  <si>
+    <t>air1.png</t>
+  </si>
+  <si>
+    <t>oz1.png</t>
+  </si>
+  <si>
+    <t>cair1.png</t>
+  </si>
+  <si>
+    <t>bair1.png</t>
+  </si>
+  <si>
+    <t>bn1.png</t>
+  </si>
+  <si>
+    <t>b1.png</t>
   </si>
 </sst>
 </file>
@@ -546,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E20EFE-B67F-440C-A476-626A60AB4D68}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,9 +593,11 @@
     <col min="4" max="4" width="8.77734375" customWidth="1"/>
     <col min="5" max="5" width="8.109375" customWidth="1"/>
     <col min="6" max="6" width="15.5546875" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,8 +619,11 @@
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -607,8 +645,11 @@
       <c r="G2" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -630,8 +671,11 @@
       <c r="G3" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -653,8 +697,11 @@
       <c r="G4" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -676,8 +723,11 @@
       <c r="G5" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -699,8 +749,11 @@
       <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -722,8 +775,11 @@
       <c r="G7" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -745,8 +801,11 @@
       <c r="G8" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -768,8 +827,11 @@
       <c r="G9" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -791,15 +853,18 @@
       <c r="G10" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>54.99</v>
       </c>
       <c r="D11" t="s">
@@ -813,6 +878,9 @@
       </c>
       <c r="G11" s="2" t="s">
         <v>39</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -821,10 +889,10 @@
     <hyperlink ref="G9" r:id="rId2" location="!searchCategory=kids/tieners/schoenen" display="https://www.footlocker.nl/nl/p/nike-air-force-1-basisschool-schoenen-7926?v=316701113504 - !searchCategory=kids/tieners/schoenen" xr:uid="{46A2DA2E-202E-428D-BD22-9B96D4784872}"/>
     <hyperlink ref="G8" r:id="rId3" location="!searchCategory=kids/kinderen/schoenen" xr:uid="{D6ECCFAD-8ED3-4A1F-BF51-0DC9DA90C13E}"/>
     <hyperlink ref="G7" r:id="rId4" location="!searchCategory=alle" xr:uid="{6BA771F6-BAB3-422A-AF93-234F6CD5C293}"/>
-    <hyperlink ref="G6" r:id="rId5" location="!searchCategory=vrouwen/schoenen/running" display="!searchCategory=vrouwen/schoenen/running" xr:uid="{95062A60-0033-4267-B22E-958A3136F1B5}"/>
+    <hyperlink ref="G6" r:id="rId5" location="!searchCategory=vrouwen/schoenen/running" xr:uid="{95062A60-0033-4267-B22E-958A3136F1B5}"/>
     <hyperlink ref="G5" r:id="rId6" location="!searchCategory=vrouwen/schoenen/casual" display="https://www.footlocker.nl/nl/p/buffalo-crevis-dames-schoenen-97731?v=315241136902 - !searchCategory=vrouwen/schoenen/casual" xr:uid="{3CC346F7-F659-4480-8383-E44C006E802F}"/>
     <hyperlink ref="G2" r:id="rId7" location="!searchCategory=heren/schoenen" display="https://www.footlocker.nl/nl/p/jordan-1-mid-heren-schoenen-49357?v=314101010404 - !searchCategory=heren/schoenen" xr:uid="{E7227B9C-7930-4013-B25A-9BCBE14E629C}"/>
-    <hyperlink ref="G4" r:id="rId8" location="!searchCategory=heren/schoenen/canvasskate" display="https://www.footlocker.nl/nl/p/vans-authentic-heren-schoenen-43758?v=314520452104 - !searchCategory=heren/schoenen/canvasskate" xr:uid="{073E643B-A882-423B-B531-4B67BBF9A05D}"/>
+    <hyperlink ref="G4" r:id="rId8" location="!searchCategory=heren/schoenen/canvasskate" xr:uid="{073E643B-A882-423B-B531-4B67BBF9A05D}"/>
     <hyperlink ref="G3" r:id="rId9" xr:uid="{CA662558-37A1-48C0-84E9-8E7D1D751590}"/>
     <hyperlink ref="G11" r:id="rId10" location="!searchCategory=kids/baby/schoenen" display="https://www.footlocker.nl/nl/p/nike-air-force-1-highness-baby-schoenen-82803?v=316160928004 - !searchCategory=kids/baby/schoenen" xr:uid="{79864D07-5CD5-489F-BF6B-48789F0BCFA9}"/>
   </hyperlinks>

</xml_diff>